<commit_message>
new functions new aliases
</commit_message>
<xml_diff>
--- a/Citrix.WEMSDK.xlsx
+++ b/Citrix.WEMSDK.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A673E96-1292-4E04-862E-2DFE3151C3D2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F380F31-48E1-4698-90B8-248261260450}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="123">
   <si>
     <t>Command</t>
   </si>
@@ -387,6 +387,9 @@
   </si>
   <si>
     <t>Cannot set password yet: need encryption algorythm (Base64 and something else)</t>
+  </si>
+  <si>
+    <t>New-WEMApp</t>
   </si>
 </sst>
 </file>
@@ -717,7 +720,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A41" sqref="A41"/>
+      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -933,6 +936,9 @@
       </c>
       <c r="B16" t="s">
         <v>17</v>
+      </c>
+      <c r="C16" t="s">
+        <v>122</v>
       </c>
       <c r="D16" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
input variable checks & fixes
</commit_message>
<xml_diff>
--- a/Citrix.WEMSDK.xlsx
+++ b/Citrix.WEMSDK.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45831992-E002-4A3A-967E-B1E3FBF762D7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1EBE1FA-C431-497F-A31A-7DAF1CF86D31}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Commands and Aliasses" sheetId="1" r:id="rId1"/>
@@ -720,7 +720,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A39" sqref="A39"/>
+      <selection pane="bottomLeft" activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1114,7 +1114,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>119</v>
+        <v>39</v>
       </c>
       <c r="B29" t="s">
         <v>104</v>
@@ -1312,7 +1312,7 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>119</v>
+        <v>39</v>
       </c>
       <c r="B44" t="s">
         <v>50</v>

</xml_diff>

<commit_message>
WEMPort function completed + cleanup
</commit_message>
<xml_diff>
--- a/Citrix.WEMSDK.xlsx
+++ b/Citrix.WEMSDK.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{601C20F3-9860-44E8-BFDE-70038A83C8AC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F07C18B3-0F10-4377-83E3-C0BE0D00AE47}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -819,7 +819,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A46" sqref="A46"/>
+      <selection pane="bottomLeft" activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1160,7 +1160,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>118</v>
+        <v>39</v>
       </c>
       <c r="B25" t="s">
         <v>100</v>
@@ -1559,7 +1559,7 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>118</v>
+        <v>39</v>
       </c>
       <c r="B52" t="s">
         <v>46</v>

</xml_diff>

<commit_message>
WEMIniFileOperation functions & cleanup
</commit_message>
<xml_diff>
--- a/Citrix.WEMSDK.xlsx
+++ b/Citrix.WEMSDK.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F07C18B3-0F10-4377-83E3-C0BE0D00AE47}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FE0847B-28D4-4886-A3A6-0F0CF4ADD47E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -819,7 +819,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A26" sqref="A26"/>
+      <selection pane="bottomLeft" activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1129,7 +1129,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>118</v>
+        <v>39</v>
       </c>
       <c r="B23" t="s">
         <v>96</v>
@@ -1528,7 +1528,7 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>118</v>
+        <v>39</v>
       </c>
       <c r="B50" t="s">
         <v>44</v>

</xml_diff>

<commit_message>
unescaped sql string fixed
</commit_message>
<xml_diff>
--- a/Citrix.WEMSDK.xlsx
+++ b/Citrix.WEMSDK.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FE0847B-28D4-4886-A3A6-0F0CF4ADD47E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55FD575B-6272-44A3-9ADA-9B4F3F849CAC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -818,8 +818,8 @@
   <dimension ref="A1:E56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A50" sqref="A50"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1087,7 +1087,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>118</v>
+        <v>39</v>
       </c>
       <c r="B20" t="s">
         <v>90</v>
@@ -1486,7 +1486,7 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>118</v>
+        <v>39</v>
       </c>
       <c r="B47" t="s">
         <v>41</v>

</xml_diff>

<commit_message>
New-WEMFIleSystemOperation function & tests
</commit_message>
<xml_diff>
--- a/Citrix.WEMSDK.xlsx
+++ b/Citrix.WEMSDK.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55FD575B-6272-44A3-9ADA-9B4F3F849CAC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DDAFECA-16D0-42A5-8DDB-3A2C975779F0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,6 +11,9 @@
     <sheet name="Commands and Aliasses" sheetId="1" r:id="rId1"/>
     <sheet name="Issues" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Commands and Aliasses'!$A$1:$E$56</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -815,11 +818,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:E56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -848,7 +852,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>39</v>
       </c>
@@ -859,7 +863,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -873,7 +877,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -884,7 +888,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>39</v>
       </c>
@@ -898,7 +902,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>39</v>
       </c>
@@ -912,7 +916,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>39</v>
       </c>
@@ -926,7 +930,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>39</v>
       </c>
@@ -940,7 +944,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>39</v>
       </c>
@@ -954,7 +958,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -971,7 +975,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>39</v>
       </c>
@@ -982,7 +986,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -996,7 +1000,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>39</v>
       </c>
@@ -1010,7 +1014,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>39</v>
       </c>
@@ -1024,7 +1028,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>39</v>
       </c>
@@ -1035,7 +1039,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>39</v>
       </c>
@@ -1049,7 +1053,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>39</v>
       </c>
@@ -1060,7 +1064,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>39</v>
       </c>
@@ -1071,7 +1075,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>39</v>
       </c>
@@ -1085,7 +1089,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>39</v>
       </c>
@@ -1127,7 +1131,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>39</v>
       </c>
@@ -1141,7 +1145,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>39</v>
       </c>
@@ -1158,7 +1162,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>39</v>
       </c>
@@ -1169,7 +1173,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>39</v>
       </c>
@@ -1183,7 +1187,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>39</v>
       </c>
@@ -1214,7 +1218,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>39</v>
       </c>
@@ -1225,7 +1229,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>39</v>
       </c>
@@ -1239,7 +1243,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>39</v>
       </c>
@@ -1256,7 +1260,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>39</v>
       </c>
@@ -1270,7 +1274,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>39</v>
       </c>
@@ -1287,7 +1291,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>39</v>
       </c>
@@ -1304,7 +1308,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>39</v>
       </c>
@@ -1321,7 +1325,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>39</v>
       </c>
@@ -1338,7 +1342,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>39</v>
       </c>
@@ -1355,7 +1359,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>39</v>
       </c>
@@ -1372,7 +1376,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>39</v>
       </c>
@@ -1386,7 +1390,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -1400,7 +1404,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>39</v>
       </c>
@@ -1417,7 +1421,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>39</v>
       </c>
@@ -1431,7 +1435,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>39</v>
       </c>
@@ -1445,7 +1449,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>39</v>
       </c>
@@ -1459,7 +1463,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>39</v>
       </c>
@@ -1470,7 +1474,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>39</v>
       </c>
@@ -1484,7 +1488,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>39</v>
       </c>
@@ -1526,7 +1530,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>39</v>
       </c>
@@ -1540,7 +1544,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>39</v>
       </c>
@@ -1557,7 +1561,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>39</v>
       </c>
@@ -1568,7 +1572,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>39</v>
       </c>
@@ -1582,7 +1586,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>39</v>
       </c>
@@ -1610,7 +1614,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>39</v>
       </c>
@@ -1622,6 +1626,13 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E56" xr:uid="{5BB291EF-653F-4FD8-900C-6852B0E4EEFE}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="In Development"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
WEMUserDSN functions completed & tests updated
</commit_message>
<xml_diff>
--- a/Citrix.WEMSDK.xlsx
+++ b/Citrix.WEMSDK.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DDAFECA-16D0-42A5-8DDB-3A2C975779F0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CEAD597-DE3B-4D22-85E8-C1AF0AF73C57}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Commands and Aliasses" sheetId="1" r:id="rId1"/>
@@ -818,12 +818,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:E56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -852,7 +851,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>39</v>
       </c>
@@ -863,7 +862,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -877,7 +876,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -888,7 +887,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>39</v>
       </c>
@@ -902,7 +901,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>39</v>
       </c>
@@ -916,7 +915,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>39</v>
       </c>
@@ -930,7 +929,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>39</v>
       </c>
@@ -944,7 +943,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>39</v>
       </c>
@@ -958,7 +957,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -975,7 +974,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>39</v>
       </c>
@@ -986,7 +985,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -1000,7 +999,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>39</v>
       </c>
@@ -1014,7 +1013,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>39</v>
       </c>
@@ -1028,7 +1027,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>39</v>
       </c>
@@ -1039,7 +1038,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>39</v>
       </c>
@@ -1053,7 +1052,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>39</v>
       </c>
@@ -1064,7 +1063,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>39</v>
       </c>
@@ -1075,7 +1074,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>39</v>
       </c>
@@ -1089,7 +1088,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>39</v>
       </c>
@@ -1119,7 +1118,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>118</v>
+        <v>39</v>
       </c>
       <c r="B22" t="s">
         <v>94</v>
@@ -1131,7 +1130,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>39</v>
       </c>
@@ -1145,7 +1144,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>39</v>
       </c>
@@ -1162,7 +1161,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>39</v>
       </c>
@@ -1173,7 +1172,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="26" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>39</v>
       </c>
@@ -1187,7 +1186,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="27" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>39</v>
       </c>
@@ -1218,7 +1217,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="29" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>39</v>
       </c>
@@ -1229,7 +1228,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="30" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>39</v>
       </c>
@@ -1243,7 +1242,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="31" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>39</v>
       </c>
@@ -1260,7 +1259,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="32" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>39</v>
       </c>
@@ -1274,7 +1273,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="33" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>39</v>
       </c>
@@ -1291,7 +1290,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="34" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>39</v>
       </c>
@@ -1308,7 +1307,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="35" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>39</v>
       </c>
@@ -1325,7 +1324,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="36" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>39</v>
       </c>
@@ -1342,7 +1341,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="37" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>39</v>
       </c>
@@ -1359,7 +1358,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="38" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>39</v>
       </c>
@@ -1376,7 +1375,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="39" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>39</v>
       </c>
@@ -1390,7 +1389,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="40" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -1404,7 +1403,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="41" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>39</v>
       </c>
@@ -1421,7 +1420,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="42" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>39</v>
       </c>
@@ -1435,7 +1434,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="43" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>39</v>
       </c>
@@ -1449,7 +1448,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="44" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>39</v>
       </c>
@@ -1463,7 +1462,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="45" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>39</v>
       </c>
@@ -1474,7 +1473,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="46" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>39</v>
       </c>
@@ -1488,7 +1487,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="47" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>39</v>
       </c>
@@ -1518,7 +1517,7 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>118</v>
+        <v>39</v>
       </c>
       <c r="B49" t="s">
         <v>43</v>
@@ -1530,7 +1529,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="50" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>39</v>
       </c>
@@ -1544,7 +1543,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="51" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>39</v>
       </c>
@@ -1561,7 +1560,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="52" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>39</v>
       </c>
@@ -1572,7 +1571,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="53" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>39</v>
       </c>
@@ -1586,7 +1585,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="54" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>39</v>
       </c>
@@ -1614,7 +1613,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="56" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>39</v>
       </c>
@@ -1626,13 +1625,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E56" xr:uid="{5BB291EF-653F-4FD8-900C-6852B0E4EEFE}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="In Development"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:E56" xr:uid="{5BB291EF-653F-4FD8-900C-6852B0E4EEFE}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Get-WEMCondition & New-WEMCondition completed
</commit_message>
<xml_diff>
--- a/Citrix.WEMSDK.xlsx
+++ b/Citrix.WEMSDK.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF83590F-955D-42E8-BCE4-E7DE69BE7C98}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4F577D6-83CF-4EB7-A003-FDFD7F0B1F25}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -14,17 +14,23 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Commands and Aliasses'!$A$1:$E$60</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="184">
   <si>
     <t>Command</t>
   </si>
@@ -503,6 +509,9 @@
     <t>Create a new Active Directory object in the WEM Database.</t>
   </si>
   <si>
+    <t>In Development</t>
+  </si>
+  <si>
     <t>Remove-WEMADObject</t>
   </si>
   <si>
@@ -525,6 +534,54 @@
   </si>
   <si>
     <t>Added Get-ActiveDirectoryName function that returns an object containing the Netbios account name. Input SID</t>
+  </si>
+  <si>
+    <t>Get-WEMCondition</t>
+  </si>
+  <si>
+    <t>Returns one or more Filter Condition objects from the WEM Database.</t>
+  </si>
+  <si>
+    <t>Set-WEMCondition</t>
+  </si>
+  <si>
+    <t>New-WEMCondition</t>
+  </si>
+  <si>
+    <t>Remove-WEMCondition</t>
+  </si>
+  <si>
+    <t>Removes a Filter Condition object from the WEM Database.</t>
+  </si>
+  <si>
+    <t>Creates a Filter Condition object from the WEM Database.</t>
+  </si>
+  <si>
+    <t>Updates a Filter Condition object from the WEM Database.</t>
+  </si>
+  <si>
+    <t>Get-WEMRule</t>
+  </si>
+  <si>
+    <t>Set-WEMRule</t>
+  </si>
+  <si>
+    <t>New-WEMRule</t>
+  </si>
+  <si>
+    <t>Remove-WEMRule</t>
+  </si>
+  <si>
+    <t>Returns one or more Filter Rule objects from the WEM Database.</t>
+  </si>
+  <si>
+    <t>Updates a Filter Rule object from the WEM Database.</t>
+  </si>
+  <si>
+    <t>Creates a Filter Rule object from the WEM Database.</t>
+  </si>
+  <si>
+    <t>Removes a Filter Rule object from the WEM Database.</t>
   </si>
 </sst>
 </file>
@@ -854,11 +911,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E60"/>
+  <dimension ref="A1:E68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A47" sqref="A47"/>
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,7 +1153,7 @@
         <v>158</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1308,10 +1365,10 @@
         <v>39</v>
       </c>
       <c r="B33" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D33" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>121</v>
@@ -1528,10 +1585,10 @@
         <v>39</v>
       </c>
       <c r="B47" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D47" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -1708,6 +1765,94 @@
       </c>
       <c r="D60" t="s">
         <v>84</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>39</v>
+      </c>
+      <c r="B61" t="s">
+        <v>168</v>
+      </c>
+      <c r="D61" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>159</v>
+      </c>
+      <c r="B62" t="s">
+        <v>170</v>
+      </c>
+      <c r="D62" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>39</v>
+      </c>
+      <c r="B63" t="s">
+        <v>171</v>
+      </c>
+      <c r="D63" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>159</v>
+      </c>
+      <c r="B64" t="s">
+        <v>172</v>
+      </c>
+      <c r="D64" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>159</v>
+      </c>
+      <c r="B65" t="s">
+        <v>176</v>
+      </c>
+      <c r="D65" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>159</v>
+      </c>
+      <c r="B66" t="s">
+        <v>177</v>
+      </c>
+      <c r="D66" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>159</v>
+      </c>
+      <c r="B67" t="s">
+        <v>178</v>
+      </c>
+      <c r="D67" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>159</v>
+      </c>
+      <c r="B68" t="s">
+        <v>179</v>
+      </c>
+      <c r="D68" t="s">
+        <v>183</v>
       </c>
     </row>
   </sheetData>
@@ -1749,30 +1894,30 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B2" t="s">
         <v>157</v>
       </c>
       <c r="C2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C3" t="s">
         <v>165</v>
       </c>
-      <c r="B3" t="s">
-        <v>159</v>
-      </c>
-      <c r="C3" t="s">
-        <v>164</v>
-      </c>
       <c r="D3" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
WEMActionGroup functions ready for testing
</commit_message>
<xml_diff>
--- a/Citrix.WEMSDK.xlsx
+++ b/Citrix.WEMSDK.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21815"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BFDE2FF-103D-4790-A847-608C9C9B6AD9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F02430E3-FF0C-4BFD-AF42-B1E6959C9B07}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="192">
   <si>
     <t>Command</t>
   </si>
@@ -606,9 +606,6 @@
   </si>
   <si>
     <t>Removes an Action Group object from the WEM Database.</t>
-  </si>
-  <si>
-    <t>In Development</t>
   </si>
 </sst>
 </file>
@@ -942,7 +939,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A72" sqref="A72"/>
+      <selection pane="bottomLeft" activeCell="A73" sqref="A73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1909,7 +1906,7 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>192</v>
+        <v>39</v>
       </c>
       <c r="B71" t="s">
         <v>186</v>

</xml_diff>

<commit_message>
added advanced settings - agent
</commit_message>
<xml_diff>
--- a/Citrix.WEMSDK.xlsx
+++ b/Citrix.WEMSDK.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBFFEF33-9CA2-4006-96A0-E29E5C163F03}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFE1EAB3-FB2F-4AD0-A4CC-FEE2FCE7B66A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12,7 +12,7 @@
     <sheet name="Issues" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Commands and Aliasses'!$A$1:$E$142</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Commands and Aliasses'!$A$1:$E$145</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="396">
   <si>
     <t>Command</t>
   </si>
@@ -1202,6 +1202,24 @@
   </si>
   <si>
     <t>TODO: Determine if all properties should be available as individual parameters to the function,Implement logic for required dependencies</t>
+  </si>
+  <si>
+    <t>Get-WEMAgentSettings</t>
+  </si>
+  <si>
+    <t>Returns a WEM Agent Settings object from the WEM Database.</t>
+  </si>
+  <si>
+    <t>Reset-WEMAgentSettings</t>
+  </si>
+  <si>
+    <t>Resets a WEM Agent Settings object in the WEM Database.</t>
+  </si>
+  <si>
+    <t>Set-WEMAgentSettings</t>
+  </si>
+  <si>
+    <t>Updates a WEM Agent Settings object in the WEM Database.</t>
   </si>
 </sst>
 </file>
@@ -1539,11 +1557,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E152"/>
+  <dimension ref="A1:E155"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D123" sqref="D123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1644,13 +1662,10 @@
         <v>37</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>25</v>
+        <v>390</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>57</v>
+        <v>391</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -1658,13 +1673,13 @@
         <v>37</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>277</v>
+        <v>4</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>288</v>
+        <v>25</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>308</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -1672,10 +1687,13 @@
         <v>37</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>162</v>
+        <v>277</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>288</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>164</v>
+        <v>308</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -1683,10 +1701,10 @@
         <v>37</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>144</v>
+        <v>162</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>145</v>
+        <v>164</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -1694,10 +1712,10 @@
         <v>37</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>5</v>
+        <v>144</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>58</v>
+        <v>145</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -1705,10 +1723,10 @@
         <v>37</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>355</v>
+        <v>5</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>352</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -1716,13 +1734,10 @@
         <v>37</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>26</v>
+        <v>355</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>59</v>
+        <v>352</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -1730,13 +1745,13 @@
         <v>37</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>278</v>
+        <v>6</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>289</v>
+        <v>26</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>309</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -1744,13 +1759,13 @@
         <v>37</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>7</v>
+        <v>278</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>27</v>
+        <v>289</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>60</v>
+        <v>309</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -1758,13 +1773,13 @@
         <v>37</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>279</v>
+        <v>7</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>290</v>
+        <v>27</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>298</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -1772,13 +1787,13 @@
         <v>37</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>8</v>
+        <v>279</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>28</v>
+        <v>290</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>61</v>
+        <v>298</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -1786,13 +1801,13 @@
         <v>37</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>280</v>
+        <v>8</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>291</v>
+        <v>28</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>299</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -1800,13 +1815,13 @@
         <v>37</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>9</v>
+        <v>280</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>29</v>
+        <v>291</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>62</v>
+        <v>299</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -1814,13 +1829,13 @@
         <v>37</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>281</v>
+        <v>9</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>292</v>
+        <v>29</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>300</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -1828,13 +1843,13 @@
         <v>37</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>10</v>
+        <v>281</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>30</v>
+        <v>292</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>63</v>
+        <v>300</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -1842,13 +1857,13 @@
         <v>37</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>282</v>
+        <v>10</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>293</v>
+        <v>30</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>301</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -1856,16 +1871,13 @@
         <v>37</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>11</v>
+        <v>282</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>31</v>
+        <v>293</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>318</v>
+        <v>301</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -1873,13 +1885,16 @@
         <v>37</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>283</v>
+        <v>11</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>294</v>
+        <v>31</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>302</v>
+        <v>64</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -1887,10 +1902,13 @@
         <v>37</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>364</v>
+        <v>283</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>294</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>365</v>
+        <v>302</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -1898,10 +1916,10 @@
         <v>37</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>12</v>
+        <v>364</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>65</v>
+        <v>365</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -1909,10 +1927,10 @@
         <v>37</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>284</v>
+        <v>12</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>303</v>
+        <v>65</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -1920,13 +1938,10 @@
         <v>37</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>13</v>
+        <v>284</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>318</v>
+        <v>303</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -1934,10 +1949,13 @@
         <v>37</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>285</v>
+        <v>13</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>304</v>
+        <v>66</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
@@ -1945,13 +1963,10 @@
         <v>37</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>32</v>
+        <v>285</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>67</v>
+        <v>304</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
@@ -1959,13 +1974,13 @@
         <v>37</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>286</v>
+        <v>14</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>295</v>
+        <v>32</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>305</v>
+        <v>67</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
@@ -1973,10 +1988,13 @@
         <v>37</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>150</v>
+        <v>286</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>295</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>154</v>
+        <v>305</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
@@ -1984,10 +2002,10 @@
         <v>37</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>351</v>
+        <v>150</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>388</v>
+        <v>154</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
@@ -1995,13 +2013,10 @@
         <v>37</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>368</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>369</v>
+        <v>351</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>370</v>
+        <v>388</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
@@ -2009,10 +2024,13 @@
         <v>37</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>362</v>
+        <v>368</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>369</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>363</v>
+        <v>370</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
@@ -2020,13 +2038,10 @@
         <v>37</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>15</v>
+        <v>362</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>318</v>
+        <v>363</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
@@ -2034,10 +2049,13 @@
         <v>37</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>287</v>
+        <v>15</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>306</v>
+        <v>68</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
@@ -2045,10 +2063,10 @@
         <v>37</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>356</v>
+        <v>287</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>357</v>
+        <v>306</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
@@ -2056,10 +2074,10 @@
         <v>37</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>16</v>
+        <v>356</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>69</v>
+        <v>357</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
@@ -2067,10 +2085,10 @@
         <v>37</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>296</v>
+        <v>16</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>307</v>
+        <v>69</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
@@ -2078,10 +2096,10 @@
         <v>37</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>157</v>
+        <v>296</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>193</v>
+        <v>307</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
@@ -2089,10 +2107,10 @@
         <v>37</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>237</v>
+        <v>157</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>323</v>
+        <v>193</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
@@ -2100,13 +2118,10 @@
         <v>37</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>330</v>
+        <v>237</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>338</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>140</v>
+        <v>323</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
@@ -2114,10 +2129,13 @@
         <v>37</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>340</v>
+        <v>330</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>345</v>
+        <v>338</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
@@ -2125,10 +2143,10 @@
         <v>37</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
@@ -2136,13 +2154,10 @@
         <v>37</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>328</v>
+        <v>348</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>329</v>
-      </c>
-      <c r="E47" s="3" t="s">
-        <v>140</v>
+        <v>349</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
@@ -2150,13 +2165,13 @@
         <v>37</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>114</v>
+        <v>328</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>320</v>
+        <v>329</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
@@ -2164,13 +2179,13 @@
         <v>37</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>205</v>
+        <v>17</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>275</v>
+        <v>114</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
@@ -2178,10 +2193,13 @@
         <v>37</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>147</v>
+        <v>205</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>275</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>189</v>
+        <v>324</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
@@ -2189,10 +2207,10 @@
         <v>37</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>18</v>
+        <v>147</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>321</v>
+        <v>189</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
@@ -2200,10 +2218,10 @@
         <v>37</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>33</v>
+        <v>321</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
@@ -2211,13 +2229,10 @@
         <v>37</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>85</v>
+        <v>19</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>101</v>
+        <v>33</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
@@ -2225,13 +2240,13 @@
         <v>37</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>206</v>
+        <v>84</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>311</v>
+        <v>85</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>166</v>
+        <v>101</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
@@ -2239,13 +2254,13 @@
         <v>37</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>86</v>
+        <v>206</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>87</v>
+        <v>311</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>102</v>
+        <v>166</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
@@ -2253,13 +2268,13 @@
         <v>37</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>207</v>
+        <v>86</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>312</v>
+        <v>87</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>167</v>
+        <v>102</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
@@ -2267,13 +2282,13 @@
         <v>37</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>88</v>
+        <v>207</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>89</v>
+        <v>312</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>103</v>
+        <v>167</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
@@ -2281,13 +2296,13 @@
         <v>37</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>208</v>
+        <v>88</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>313</v>
+        <v>89</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>168</v>
+        <v>103</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
@@ -2295,13 +2310,13 @@
         <v>37</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>90</v>
+        <v>208</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>91</v>
+        <v>313</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>104</v>
+        <v>168</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
@@ -2309,13 +2324,13 @@
         <v>37</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>209</v>
+        <v>90</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>314</v>
+        <v>91</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>169</v>
+        <v>104</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
@@ -2323,13 +2338,13 @@
         <v>37</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>92</v>
+        <v>209</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>93</v>
+        <v>314</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>105</v>
+        <v>169</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
@@ -2337,13 +2352,13 @@
         <v>37</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>210</v>
+        <v>92</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>315</v>
+        <v>93</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>170</v>
+        <v>105</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
@@ -2351,16 +2366,13 @@
         <v>37</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>94</v>
+        <v>210</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>95</v>
+        <v>315</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="E63" s="2" t="s">
-        <v>310</v>
+        <v>170</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
@@ -2368,13 +2380,16 @@
         <v>37</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>211</v>
+        <v>94</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>316</v>
+        <v>95</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>171</v>
+        <v>106</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
@@ -2382,10 +2397,13 @@
         <v>37</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>96</v>
+        <v>211</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>316</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>107</v>
+        <v>171</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
@@ -2393,10 +2411,10 @@
         <v>37</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>212</v>
+        <v>96</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>172</v>
+        <v>107</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
@@ -2404,13 +2422,10 @@
         <v>37</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>20</v>
+        <v>212</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>322</v>
-      </c>
-      <c r="E67" s="2" t="s">
-        <v>310</v>
+        <v>172</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
@@ -2418,10 +2433,13 @@
         <v>37</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>213</v>
+        <v>20</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>325</v>
+        <v>322</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
@@ -2429,16 +2447,10 @@
         <v>37</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>98</v>
+        <v>213</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="E69" s="2" t="s">
-        <v>116</v>
+        <v>325</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
@@ -2446,13 +2458,16 @@
         <v>37</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>214</v>
+        <v>97</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>317</v>
+        <v>98</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>173</v>
+        <v>108</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
@@ -2460,10 +2475,13 @@
         <v>37</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>152</v>
+        <v>214</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>317</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
@@ -2471,13 +2489,10 @@
         <v>37</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>99</v>
+        <v>152</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="E72" s="2" t="s">
-        <v>310</v>
+        <v>191</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
@@ -2485,10 +2500,13 @@
         <v>37</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>215</v>
+        <v>99</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>174</v>
+        <v>109</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
@@ -2496,10 +2514,10 @@
         <v>37</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>100</v>
+        <v>215</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>110</v>
+        <v>174</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
@@ -2507,10 +2525,10 @@
         <v>37</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>216</v>
+        <v>100</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>175</v>
+        <v>110</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
@@ -2518,13 +2536,10 @@
         <v>37</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>21</v>
+        <v>216</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="E76" s="2" t="s">
-        <v>115</v>
+        <v>175</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
@@ -2532,10 +2547,10 @@
         <v>37</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>159</v>
+        <v>21</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>161</v>
+        <v>70</v>
       </c>
       <c r="E77" s="2" t="s">
         <v>115</v>
@@ -2546,10 +2561,10 @@
         <v>37</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>239</v>
+        <v>159</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>240</v>
+        <v>161</v>
       </c>
       <c r="E78" s="2" t="s">
         <v>115</v>
@@ -2560,12 +2575,12 @@
         <v>37</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>332</v>
+        <v>239</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>339</v>
-      </c>
-      <c r="E79" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="E79" s="2" t="s">
         <v>115</v>
       </c>
     </row>
@@ -2574,10 +2589,13 @@
         <v>37</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>346</v>
+        <v>339</v>
+      </c>
+      <c r="E80" s="3" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
@@ -2585,13 +2603,10 @@
         <v>37</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>331</v>
+        <v>341</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>333</v>
-      </c>
-      <c r="E81" s="3" t="s">
-        <v>115</v>
+        <v>346</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
@@ -2599,15 +2614,12 @@
         <v>37</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="C82" s="2" t="s">
-        <v>117</v>
+        <v>331</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="E82" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="E82" s="3" t="s">
         <v>115</v>
       </c>
     </row>
@@ -2616,13 +2628,13 @@
         <v>37</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>217</v>
+        <v>137</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>229</v>
+        <v>117</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>238</v>
+        <v>136</v>
       </c>
       <c r="E83" s="2" t="s">
         <v>115</v>
@@ -2633,10 +2645,13 @@
         <v>37</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>163</v>
+        <v>217</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>229</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>165</v>
+        <v>238</v>
       </c>
       <c r="E84" s="2" t="s">
         <v>115</v>
@@ -2647,13 +2662,13 @@
         <v>37</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>148</v>
+        <v>163</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>149</v>
+        <v>165</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>319</v>
+        <v>115</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
@@ -2661,13 +2676,13 @@
         <v>37</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>22</v>
+        <v>148</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>176</v>
+        <v>149</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>115</v>
+        <v>319</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
@@ -2675,13 +2690,10 @@
         <v>37</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="C87" s="2" t="s">
-        <v>230</v>
+        <v>22</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>194</v>
+        <v>176</v>
       </c>
       <c r="E87" s="2" t="s">
         <v>115</v>
@@ -2692,13 +2704,13 @@
         <v>37</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>118</v>
+        <v>218</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>119</v>
+        <v>230</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>177</v>
+        <v>194</v>
       </c>
       <c r="E88" s="2" t="s">
         <v>115</v>
@@ -2709,13 +2721,13 @@
         <v>37</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E89" s="2" t="s">
         <v>115</v>
@@ -2726,13 +2738,13 @@
         <v>37</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>219</v>
+        <v>120</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>231</v>
+        <v>121</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>195</v>
+        <v>178</v>
       </c>
       <c r="E90" s="2" t="s">
         <v>115</v>
@@ -2743,13 +2755,13 @@
         <v>37</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>122</v>
+        <v>219</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>123</v>
+        <v>231</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="E91" s="2" t="s">
         <v>115</v>
@@ -2760,13 +2772,13 @@
         <v>37</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>220</v>
+        <v>122</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>232</v>
+        <v>123</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>196</v>
+        <v>179</v>
       </c>
       <c r="E92" s="2" t="s">
         <v>115</v>
@@ -2777,13 +2789,13 @@
         <v>37</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>124</v>
+        <v>220</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>125</v>
+        <v>232</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="E93" s="2" t="s">
         <v>115</v>
@@ -2794,13 +2806,13 @@
         <v>37</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>221</v>
+        <v>124</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>233</v>
+        <v>125</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>197</v>
+        <v>180</v>
       </c>
       <c r="E94" s="2" t="s">
         <v>115</v>
@@ -2811,13 +2823,13 @@
         <v>37</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>126</v>
+        <v>221</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>127</v>
+        <v>233</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>181</v>
+        <v>197</v>
       </c>
       <c r="E95" s="2" t="s">
         <v>115</v>
@@ -2828,13 +2840,13 @@
         <v>37</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>222</v>
+        <v>126</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>234</v>
+        <v>127</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>198</v>
+        <v>181</v>
       </c>
       <c r="E96" s="2" t="s">
         <v>115</v>
@@ -2845,13 +2857,13 @@
         <v>37</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>128</v>
+        <v>222</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>129</v>
+        <v>234</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>182</v>
+        <v>198</v>
       </c>
       <c r="E97" s="2" t="s">
         <v>115</v>
@@ -2862,13 +2874,13 @@
         <v>37</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>223</v>
+        <v>128</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>235</v>
+        <v>129</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>199</v>
+        <v>182</v>
       </c>
       <c r="E98" s="2" t="s">
         <v>115</v>
@@ -2879,10 +2891,13 @@
         <v>37</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>130</v>
+        <v>223</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>235</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>183</v>
+        <v>199</v>
       </c>
       <c r="E99" s="2" t="s">
         <v>115</v>
@@ -2893,10 +2908,10 @@
         <v>37</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>224</v>
+        <v>130</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>200</v>
+        <v>183</v>
       </c>
       <c r="E100" s="2" t="s">
         <v>115</v>
@@ -2907,10 +2922,10 @@
         <v>37</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>131</v>
+        <v>224</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>184</v>
+        <v>200</v>
       </c>
       <c r="E101" s="2" t="s">
         <v>115</v>
@@ -2921,10 +2936,10 @@
         <v>37</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>225</v>
+        <v>131</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>201</v>
+        <v>184</v>
       </c>
       <c r="E102" s="2" t="s">
         <v>115</v>
@@ -2935,13 +2950,10 @@
         <v>37</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="C103" s="2" t="s">
-        <v>133</v>
+        <v>225</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>185</v>
+        <v>201</v>
       </c>
       <c r="E103" s="2" t="s">
         <v>115</v>
@@ -2952,13 +2964,13 @@
         <v>37</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>226</v>
+        <v>132</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>236</v>
+        <v>133</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>202</v>
+        <v>185</v>
       </c>
       <c r="E104" s="2" t="s">
         <v>115</v>
@@ -2969,10 +2981,13 @@
         <v>37</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>153</v>
+        <v>226</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>236</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>155</v>
+        <v>202</v>
       </c>
       <c r="E105" s="2" t="s">
         <v>115</v>
@@ -2983,10 +2998,10 @@
         <v>37</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>134</v>
+        <v>153</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>186</v>
+        <v>155</v>
       </c>
       <c r="E106" s="2" t="s">
         <v>115</v>
@@ -2997,10 +3012,10 @@
         <v>37</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>227</v>
+        <v>134</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>203</v>
+        <v>186</v>
       </c>
       <c r="E107" s="2" t="s">
         <v>115</v>
@@ -3011,10 +3026,10 @@
         <v>37</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>135</v>
+        <v>227</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="E108" s="2" t="s">
         <v>115</v>
@@ -3025,10 +3040,10 @@
         <v>37</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>228</v>
+        <v>135</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>204</v>
+        <v>187</v>
       </c>
       <c r="E109" s="2" t="s">
         <v>115</v>
@@ -3039,10 +3054,10 @@
         <v>37</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>374</v>
+        <v>228</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>382</v>
+        <v>204</v>
       </c>
       <c r="E110" s="2" t="s">
         <v>115</v>
@@ -3053,10 +3068,10 @@
         <v>37</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>375</v>
+        <v>392</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>383</v>
+        <v>393</v>
       </c>
       <c r="E111" s="2" t="s">
         <v>115</v>
@@ -3067,10 +3082,10 @@
         <v>37</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="E112" s="2" t="s">
         <v>115</v>
@@ -3081,13 +3096,10 @@
         <v>37</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>377</v>
-      </c>
-      <c r="C113" s="2" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="E113" s="2" t="s">
         <v>115</v>
@@ -3098,10 +3110,10 @@
         <v>37</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="E114" s="2" t="s">
         <v>115</v>
@@ -3112,10 +3124,13 @@
         <v>37</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>380</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>381</v>
+        <v>385</v>
       </c>
       <c r="E115" s="2" t="s">
         <v>115</v>
@@ -3126,10 +3141,13 @@
         <v>37</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>158</v>
+        <v>379</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>192</v>
+        <v>386</v>
+      </c>
+      <c r="E116" s="2" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
@@ -3137,10 +3155,13 @@
         <v>37</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>261</v>
+        <v>378</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>262</v>
+        <v>381</v>
+      </c>
+      <c r="E117" s="2" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
@@ -3148,10 +3169,10 @@
         <v>37</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>342</v>
+        <v>158</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>347</v>
+        <v>192</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
@@ -3159,10 +3180,10 @@
         <v>37</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>334</v>
+        <v>261</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>335</v>
+        <v>262</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.2">
@@ -3170,13 +3191,10 @@
         <v>37</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C120" s="2" t="s">
-        <v>35</v>
+        <v>342</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>71</v>
+        <v>347</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.2">
@@ -3184,24 +3202,24 @@
         <v>37</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="C121" s="2" t="s">
-        <v>253</v>
+        <v>334</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A122" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>146</v>
+        <v>394</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>188</v>
+        <v>395</v>
+      </c>
+      <c r="E122" s="3" t="s">
+        <v>389</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.2">
@@ -3209,24 +3227,27 @@
         <v>37</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
+      </c>
+      <c r="C123" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>353</v>
+        <v>241</v>
+      </c>
+      <c r="C124" s="2" t="s">
+        <v>253</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>354</v>
-      </c>
-      <c r="E124" s="3" t="s">
-        <v>389</v>
+        <v>274</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.2">
@@ -3234,13 +3255,10 @@
         <v>37</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C125" s="2" t="s">
-        <v>49</v>
+        <v>146</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>81</v>
+        <v>188</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.2">
@@ -3248,27 +3266,24 @@
         <v>37</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="C126" s="2" t="s">
-        <v>254</v>
+        <v>24</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A127" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C127" s="2" t="s">
-        <v>50</v>
+        <v>353</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>82</v>
+        <v>354</v>
+      </c>
+      <c r="E127" s="3" t="s">
+        <v>389</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.2">
@@ -3276,13 +3291,13 @@
         <v>37</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>243</v>
+        <v>38</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>255</v>
+        <v>49</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>263</v>
+        <v>81</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.2">
@@ -3290,13 +3305,13 @@
         <v>37</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>40</v>
+        <v>242</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>51</v>
+        <v>254</v>
       </c>
       <c r="D129" s="2" t="s">
-        <v>73</v>
+        <v>273</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.2">
@@ -3304,13 +3319,13 @@
         <v>37</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>244</v>
+        <v>39</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>256</v>
+        <v>50</v>
       </c>
       <c r="D130" s="2" t="s">
-        <v>264</v>
+        <v>82</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.2">
@@ -3318,13 +3333,13 @@
         <v>37</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>41</v>
+        <v>243</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>52</v>
+        <v>255</v>
       </c>
       <c r="D131" s="2" t="s">
-        <v>74</v>
+        <v>263</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.2">
@@ -3332,13 +3347,13 @@
         <v>37</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>245</v>
+        <v>40</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>257</v>
+        <v>51</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>265</v>
+        <v>73</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.2">
@@ -3346,13 +3361,13 @@
         <v>37</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>42</v>
+        <v>244</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>53</v>
+        <v>256</v>
       </c>
       <c r="D133" s="2" t="s">
-        <v>83</v>
+        <v>264</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.2">
@@ -3360,13 +3375,13 @@
         <v>37</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>246</v>
+        <v>41</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>258</v>
+        <v>52</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>266</v>
+        <v>74</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.2">
@@ -3374,16 +3389,13 @@
         <v>37</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>43</v>
+        <v>245</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>54</v>
+        <v>257</v>
       </c>
       <c r="D135" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E135" s="2" t="s">
-        <v>310</v>
+        <v>265</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.2">
@@ -3391,27 +3403,27 @@
         <v>37</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>247</v>
+        <v>42</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>259</v>
+        <v>53</v>
       </c>
       <c r="D136" s="2" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="137" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A137" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>366</v>
+        <v>246</v>
+      </c>
+      <c r="C137" s="2" t="s">
+        <v>258</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>367</v>
-      </c>
-      <c r="E137" s="3" t="s">
-        <v>389</v>
+        <v>266</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.2">
@@ -3419,10 +3431,16 @@
         <v>37</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
+      </c>
+      <c r="C138" s="2" t="s">
+        <v>54</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
+      </c>
+      <c r="E138" s="2" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.2">
@@ -3430,24 +3448,27 @@
         <v>37</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
+      </c>
+      <c r="C139" s="2" t="s">
+        <v>259</v>
       </c>
       <c r="D139" s="2" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A140" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>45</v>
+        <v>366</v>
       </c>
       <c r="D140" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E140" s="2" t="s">
-        <v>310</v>
+        <v>367</v>
+      </c>
+      <c r="E140" s="3" t="s">
+        <v>389</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.2">
@@ -3455,10 +3476,10 @@
         <v>37</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>249</v>
+        <v>44</v>
       </c>
       <c r="D141" s="2" t="s">
-        <v>269</v>
+        <v>76</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.2">
@@ -3466,13 +3487,10 @@
         <v>37</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C142" s="2" t="s">
-        <v>55</v>
+        <v>248</v>
       </c>
       <c r="D142" s="2" t="s">
-        <v>78</v>
+        <v>268</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.2">
@@ -3480,13 +3498,13 @@
         <v>37</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="C143" s="2" t="s">
-        <v>260</v>
+        <v>45</v>
       </c>
       <c r="D143" s="2" t="s">
-        <v>270</v>
+        <v>77</v>
+      </c>
+      <c r="E143" s="2" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.2">
@@ -3494,80 +3512,80 @@
         <v>37</v>
       </c>
       <c r="B144" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="D144" s="2" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A145" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B145" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C145" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D145" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A146" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B146" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="C146" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="D146" s="2" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A147" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B147" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="D144" s="2" t="s">
+      <c r="D147" s="2" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="145" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A145" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B145" s="2" t="s">
+    <row r="148" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A148" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B148" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="D145" s="2" t="s">
+      <c r="D148" s="2" t="s">
         <v>387</v>
       </c>
-      <c r="E145" s="3" t="s">
+      <c r="E148" s="3" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="146" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A146" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B146" s="2" t="s">
+    <row r="149" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A149" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B149" s="2" t="s">
         <v>371</v>
       </c>
-      <c r="C146" s="2" t="s">
+      <c r="C149" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="D146" s="2" t="s">
+      <c r="D149" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="E146" s="3" t="s">
+      <c r="E149" s="3" t="s">
         <v>389</v>
-      </c>
-    </row>
-    <row r="147" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A147" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B147" s="2" t="s">
-        <v>360</v>
-      </c>
-      <c r="D147" s="2" t="s">
-        <v>361</v>
-      </c>
-      <c r="E147" s="3" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A148" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B148" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D148" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E148" s="2" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A149" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B149" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="D149" s="2" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="150" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
@@ -3575,10 +3593,10 @@
         <v>37</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="D150" s="2" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="E150" s="3" t="s">
         <v>389</v>
@@ -3589,10 +3607,13 @@
         <v>37</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D151" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
+      </c>
+      <c r="E151" s="2" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.2">
@@ -3600,16 +3621,52 @@
         <v>37</v>
       </c>
       <c r="B152" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="D152" s="2" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A153" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B153" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="D153" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="E153" s="3" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A154" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B154" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D154" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A155" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B155" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="D152" s="2" t="s">
+      <c r="D155" s="2" t="s">
         <v>272</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E142" xr:uid="{5BB291EF-653F-4FD8-900C-6852B0E4EEFE}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E152">
-      <sortCondition ref="B1:B142"/>
+  <autoFilter ref="A1:E145" xr:uid="{5BB291EF-653F-4FD8-900C-6852B0E4EEFE}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E155">
+      <sortCondition ref="B1:B145"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Shortcut processing in Import-VUEMActionsFromGpo
</commit_message>
<xml_diff>
--- a/Citrix.WEMSDK.xlsx
+++ b/Citrix.WEMSDK.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0B52D43-9052-489F-97DD-3331DCFC54D6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3008864A-39D8-4D44-9954-B012C8E9B3DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Commands and Aliasses" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="425">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="426">
   <si>
     <t>Command</t>
   </si>
@@ -1313,6 +1313,9 @@
   </si>
   <si>
     <t>Returns WEM System Monitoring Settings from the WEM Database.</t>
+  </si>
+  <si>
+    <t>TODO: Consider different output so filtering is possible. Output is now a hashtable with all the items.</t>
   </si>
 </sst>
 </file>
@@ -1653,8 +1656,8 @@
   <dimension ref="A1:E167"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2218,6 +2221,9 @@
       </c>
       <c r="D44" s="2" t="s">
         <v>399</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>425</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>